<commit_message>
fitur upload excel product
</commit_message>
<xml_diff>
--- a/public/downloadexample/example.xlsx
+++ b/public/downloadexample/example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\laravel-kasir\public\downloadexample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>total_stock</t>
   </si>
@@ -50,23 +50,47 @@
     <t>gersik</t>
   </si>
   <si>
-    <t>saus abc</t>
-  </si>
-  <si>
-    <t>minyak wijen</t>
-  </si>
-  <si>
     <t>kebutuhan pokok</t>
   </si>
   <si>
     <t>sayur</t>
+  </si>
+  <si>
+    <t>satuan_berat_item</t>
+  </si>
+  <si>
+    <t>harga_jual</t>
+  </si>
+  <si>
+    <t>subname</t>
+  </si>
+  <si>
+    <t>saus  MAYONES</t>
+  </si>
+  <si>
+    <t>minyak RAJA RASA</t>
+  </si>
+  <si>
+    <t>selada air</t>
+  </si>
+  <si>
+    <t>mojokerto</t>
+  </si>
+  <si>
+    <t>melon</t>
+  </si>
+  <si>
+    <t>buah</t>
+  </si>
+  <si>
+    <t>tepung segitiga biru</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,13 +106,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,9 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,10 +441,10 @@
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="45.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -422,19 +463,28 @@
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>45000</v>
@@ -445,25 +495,109 @@
       <c r="F2">
         <v>400</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>76000</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>21000</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>450</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>13000</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>700</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>7500</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>31000</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>470</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>45000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>